<commit_message>
better makefile dependency resolution
</commit_message>
<xml_diff>
--- a/project/excel/synbio_schema.xlsx
+++ b/project/excel/synbio_schema.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="13" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Database" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modification" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organism" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PartsSequence" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Strain" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Database1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modification1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organism1" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PartsSequence1" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person1" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Strain1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Database" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Modification" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Organism" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PartsSequence" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Person" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Strain" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Database1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Modification1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Organism1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PartsSequence1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Person1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Strain1" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -472,88 +470,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>NamedThing_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Organism_abbreviation</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Organism_comment</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Organism_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Organism_special_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Organism_species_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Organism_species_ncbi_taxon_number</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Organism_strain_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -644,7 +560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -705,13 +621,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,77 +638,97 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>genome_accessions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biosample_accessions</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>bio_safety_level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>funding_source</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>genotype_phenotype</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_parts</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>host_organism</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>Strain_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bio_safety_level</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>funding_source</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>genotype_phenotype</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>intellectual_property</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>principal_investigator</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>references</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>selection_markers</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_parts</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>host_organism</t>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>external_urls</t>
         </is>
       </c>
     </row>
@@ -970,7 +906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,7 +917,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>NamedThing_id</t>
+          <t>Organism_abbreviation</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Organism_comment</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Organism_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Organism_special_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Organism_species_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Organism_species_ncbi_taxon_number</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Organism_strain_value</t>
         </is>
       </c>
     </row>
@@ -991,6 +957,484 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>PartsSequence_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PartsSequence_associated_part</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>date_added</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>go_term_ids</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>go_term_labels</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>match_ec_numbers</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>match_gene_symbols_etc</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>match_names</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nt_sequence</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>other_accessions</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>scientific_names</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>seq_name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>seq_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>taxon_ids</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>uniprot_accessions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="M2:M1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"deletion,sequence,insertion,flank1,flank2"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"deletion,sequence,insertion,flank1,flank2"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Person_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Person_date_joined</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Person_email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Person_first_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Person_is_staff</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Person_is_superuser</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Person_last_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Person_username</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>genome_accessions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>biosample_accessions</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>bio_safety_level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>funding_source</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>genotype_phenotype</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_parts</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>host_organism</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Strain_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intellectual_property</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>principal_investigator</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>selection_markers</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>external_urls</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Level 1,Level 2"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"IARPA-FELIX"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"In Progress,Abandoned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Level 1,Level 2"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"IARPA-FELIX"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"In Progress,Abandoned"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Database_modification_set</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Database_organism_set</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Database_person_set</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Database_sequence_set</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Database_strain_set</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Modification_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Modification_aa_change</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Modification_bio_safety_level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Modification_category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Modification_creator</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Modification_descriptor</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Modification_el_name_long</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Modification_el_name_short</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Modification_element_organism</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Modification_modification_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Modification_modifications_genes</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Modification_notes</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Modification_position</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Modification_principal_investigator</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Modification_size_bp</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Modification_status</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Modification_subcategory_size</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Modification_curated_gene_symbols</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>curated_protein_name</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>curated_enzyme_name</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>curated_uniprot_accession</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>part_ofs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1044,462 +1488,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>PartsSequence_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>PartsSequence_associated_part</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>date_added</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>go_term_ids</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>go_term_labels</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>match_ec_numbers</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>match_gene_symbols_etc</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>match_names</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>nt_sequence</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>other_accessions</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>scientific_names</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>seq_name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>seq_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>taxon_ids</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>uniprot_accessions</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="M2:M1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"deletion,sequence,insertion,flank1,flank2"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"deletion,sequence,insertion,flank1,flank2"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Person_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Person_date_joined</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Person_email</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Person_first_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Person_is_staff</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Person_is_superuser</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Person_last_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Person_username</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Strain_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bio_safety_level</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>funding_source</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>genotype_phenotype</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intellectual_property</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>principal_investigator</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>references</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>summary</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_parts</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>host_organism</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"Level 1,Level 2"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"IARPA-FELIX"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L2:L1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"In Progress,Abandoned"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"Level 1,Level 2"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"IARPA-FELIX"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L2:L1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"In Progress,Abandoned"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Database_modification_set</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Database_organism_set</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Database_person_set</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Database_sequence_set</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Database_strain_set</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Modification_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Modification_aa_change</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Modification_bio_safety_level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Modification_category</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Modification_creator</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Modification_descriptor</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Modification_el_name_long</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Modification_el_name_short</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Modification_element_organism</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Modification_modification_type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Modification_modifications_genes</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Modification_notes</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Modification_position</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Modification_principal_investigator</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Modification_size_bp</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Modification_status</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Modification_subcategory_size</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Modification_curated_gene_symbols</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>curated_protein_name</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>curated_enzyme_name</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>curated_uniprot_accession</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>part_ofs</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>